<commit_message>
git diff 1234.xlsx is working now.
</commit_message>
<xml_diff>
--- a/1234.xlsx
+++ b/1234.xlsx
@@ -24,6 +24,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,7 +109,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -118,7 +119,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>2</v>

</xml_diff>